<commit_message>
estimaciones DT (al finnn )
</commit_message>
<xml_diff>
--- a/input/data/dt/CAE_DT_armonizado.xlsx
+++ b/input/data/dt/CAE_DT_armonizado.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\proyecto_sindicalizacion\input\data\dt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB16E66-E1C3-42C8-AAC6-A0838FCD3E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662F9BCA-8C78-4E1A-9479-35D85F686AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-1335" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -814,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E90" sqref="E90"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1441,7 +1441,7 @@
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="8" t="s">
         <v>38</v>
       </c>
       <c r="C37">
@@ -1570,7 +1570,7 @@
         <v>20</v>
       </c>
       <c r="E44">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
arrriba unificado final, falta 2020:2023
</commit_message>
<xml_diff>
--- a/input/data/dt/CAE_DT_armonizado.xlsx
+++ b/input/data/dt/CAE_DT_armonizado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\proyecto_sindicalizacion\input\data\dt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662F9BCA-8C78-4E1A-9479-35D85F686AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B13DF57-7D7B-44CA-8E5B-C6330B0B482C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -814,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1407,14 +1407,14 @@
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C35">
         <v>8498</v>
       </c>
       <c r="D35">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E35">
         <v>35</v>

</xml_diff>

<commit_message>
avance casi listo falta 2023
</commit_message>
<xml_diff>
--- a/input/data/dt/CAE_DT_armonizado.xlsx
+++ b/input/data/dt/CAE_DT_armonizado.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\proyecto_sindicalizacion\input\data\dt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C5FEE7-1C75-4DC0-855C-7D8C55EE3BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF4153E-1904-49F3-A424-FAA61ED41CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-1335" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19200" yWindow="-1215" windowWidth="19200" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="124">
   <si>
     <t>id_cae2</t>
   </si>
@@ -389,6 +389,9 @@
   </si>
   <si>
     <t>ID2</t>
+  </si>
+  <si>
+    <t>codigoactividad</t>
   </si>
 </sst>
 </file>
@@ -875,20 +878,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G90"/>
+  <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E90" sqref="E90"/>
+    <sheetView tabSelected="1" topLeftCell="B34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="124.08984375" customWidth="1"/>
-    <col min="4" max="5" width="11.453125" customWidth="1"/>
-    <col min="6" max="6" width="13.26953125" customWidth="1"/>
+    <col min="4" max="6" width="11.453125" customWidth="1"/>
+    <col min="7" max="7" width="13.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -905,13 +908,16 @@
         <v>122</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -927,14 +933,17 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -950,14 +959,17 @@
       <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -973,14 +985,17 @@
       <c r="E4">
         <v>3</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -996,14 +1011,17 @@
       <c r="E5">
         <v>4</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1019,14 +1037,17 @@
       <c r="E6">
         <v>4</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1042,14 +1063,17 @@
       <c r="E7">
         <v>4</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1065,14 +1089,17 @@
       <c r="E8">
         <v>4</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1088,14 +1115,17 @@
       <c r="E9">
         <v>4</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1111,14 +1141,17 @@
       <c r="E10">
         <v>4</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10">
+        <v>9</v>
+      </c>
+      <c r="G10" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1137,11 +1170,14 @@
       <c r="F11">
         <v>10</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1160,11 +1196,14 @@
       <c r="F12">
         <v>11</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12">
+        <v>11</v>
+      </c>
+      <c r="H12" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1183,11 +1222,14 @@
       <c r="F13">
         <v>12</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13">
+        <v>12</v>
+      </c>
+      <c r="H13" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1204,13 +1246,16 @@
         <v>6</v>
       </c>
       <c r="F14">
+        <v>13</v>
+      </c>
+      <c r="G14">
         <v>14</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1229,11 +1274,14 @@
       <c r="F15">
         <v>14</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15">
+        <v>14</v>
+      </c>
+      <c r="H15" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1250,13 +1298,16 @@
         <v>6</v>
       </c>
       <c r="F16">
+        <v>15</v>
+      </c>
+      <c r="G16">
         <v>14</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1275,11 +1326,14 @@
       <c r="F17">
         <v>16</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17">
+        <v>16</v>
+      </c>
+      <c r="H17" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1298,11 +1352,14 @@
       <c r="F18">
         <v>17</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18">
+        <v>17</v>
+      </c>
+      <c r="H18" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1321,11 +1378,14 @@
       <c r="F19">
         <v>18</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19">
+        <v>18</v>
+      </c>
+      <c r="H19" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1344,11 +1404,14 @@
       <c r="F20">
         <v>19</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20">
+        <v>19</v>
+      </c>
+      <c r="H20" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1367,11 +1430,14 @@
       <c r="F21">
         <v>20</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21">
+        <v>20</v>
+      </c>
+      <c r="H21" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1390,11 +1456,14 @@
       <c r="F22">
         <v>21</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22">
+        <v>21</v>
+      </c>
+      <c r="H22" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1413,11 +1482,14 @@
       <c r="F23">
         <v>22</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23">
+        <v>22</v>
+      </c>
+      <c r="H23" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1436,11 +1508,14 @@
       <c r="F24">
         <v>23</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24">
+        <v>23</v>
+      </c>
+      <c r="H24" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1459,11 +1534,14 @@
       <c r="F25">
         <v>24</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25">
+        <v>24</v>
+      </c>
+      <c r="H25" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1482,11 +1560,14 @@
       <c r="F26">
         <v>25</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26">
+        <v>25</v>
+      </c>
+      <c r="H26" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1503,13 +1584,16 @@
         <v>10</v>
       </c>
       <c r="F27">
+        <v>26</v>
+      </c>
+      <c r="G27">
         <v>27</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1528,11 +1612,14 @@
       <c r="F28">
         <v>27</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28">
+        <v>27</v>
+      </c>
+      <c r="H28" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1549,13 +1636,16 @@
         <v>10</v>
       </c>
       <c r="F29">
+        <v>28</v>
+      </c>
+      <c r="G29">
         <v>27</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1572,13 +1662,16 @@
         <v>10</v>
       </c>
       <c r="F30">
+        <v>29</v>
+      </c>
+      <c r="G30">
         <v>30</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1597,11 +1690,14 @@
       <c r="F31">
         <v>30</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31">
+        <v>30</v>
+      </c>
+      <c r="H31" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1620,11 +1716,14 @@
       <c r="F32">
         <v>31</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G32">
+        <v>31</v>
+      </c>
+      <c r="H32" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1643,11 +1742,14 @@
       <c r="F33">
         <v>32</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G33">
+        <v>32</v>
+      </c>
+      <c r="H33" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1666,11 +1768,14 @@
       <c r="F34">
         <v>33</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G34">
+        <v>33</v>
+      </c>
+      <c r="H34" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1689,11 +1794,14 @@
       <c r="F35">
         <v>35</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G35">
+        <v>35</v>
+      </c>
+      <c r="H35" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1712,11 +1820,14 @@
       <c r="F36">
         <v>36</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36">
+        <v>36</v>
+      </c>
+      <c r="H36" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1735,11 +1846,14 @@
       <c r="F37">
         <v>37</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G37">
+        <v>37</v>
+      </c>
+      <c r="H37" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1758,11 +1872,14 @@
       <c r="F38">
         <v>38</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G38">
+        <v>38</v>
+      </c>
+      <c r="H38" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1781,11 +1898,14 @@
       <c r="F39">
         <v>39</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G39">
+        <v>39</v>
+      </c>
+      <c r="H39" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1804,11 +1924,14 @@
       <c r="F40">
         <v>41</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40">
+        <v>41</v>
+      </c>
+      <c r="H40" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1827,11 +1950,14 @@
       <c r="F41">
         <v>42</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G41">
+        <v>42</v>
+      </c>
+      <c r="H41" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1850,11 +1976,14 @@
       <c r="F42">
         <v>43</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G42">
+        <v>43</v>
+      </c>
+      <c r="H42" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1873,11 +2002,14 @@
       <c r="F43">
         <v>45</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G43">
+        <v>45</v>
+      </c>
+      <c r="H43" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1894,13 +2026,16 @@
         <v>15</v>
       </c>
       <c r="F44">
+        <v>46</v>
+      </c>
+      <c r="G44">
         <v>47</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1917,13 +2052,16 @@
         <v>16</v>
       </c>
       <c r="F45">
+        <v>47</v>
+      </c>
+      <c r="G45">
         <v>48</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1942,11 +2080,14 @@
       <c r="F46">
         <v>49</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G46">
+        <v>49</v>
+      </c>
+      <c r="H46" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1965,11 +2106,14 @@
       <c r="F47">
         <v>50</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G47">
+        <v>50</v>
+      </c>
+      <c r="H47" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1988,11 +2132,14 @@
       <c r="F48">
         <v>51</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G48">
+        <v>51</v>
+      </c>
+      <c r="H48" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2011,11 +2158,14 @@
       <c r="F49">
         <v>52</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G49">
+        <v>52</v>
+      </c>
+      <c r="H49" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2034,11 +2184,14 @@
       <c r="F50">
         <v>53</v>
       </c>
-      <c r="G50" t="s">
+      <c r="G50">
+        <v>53</v>
+      </c>
+      <c r="H50" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2057,11 +2210,14 @@
       <c r="F51">
         <v>55</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G51">
+        <v>55</v>
+      </c>
+      <c r="H51" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2080,11 +2236,14 @@
       <c r="F52">
         <v>56</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G52">
+        <v>56</v>
+      </c>
+      <c r="H52" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2103,11 +2262,14 @@
       <c r="F53">
         <v>58</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G53">
+        <v>58</v>
+      </c>
+      <c r="H53" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2126,11 +2288,14 @@
       <c r="F54">
         <v>59</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G54">
+        <v>59</v>
+      </c>
+      <c r="H54" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2149,11 +2314,14 @@
       <c r="F55">
         <v>60</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G55">
+        <v>60</v>
+      </c>
+      <c r="H55" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2172,11 +2340,14 @@
       <c r="F56">
         <v>61</v>
       </c>
-      <c r="G56" t="s">
+      <c r="G56">
+        <v>61</v>
+      </c>
+      <c r="H56" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2195,11 +2366,14 @@
       <c r="F57">
         <v>62</v>
       </c>
-      <c r="G57" t="s">
+      <c r="G57">
+        <v>62</v>
+      </c>
+      <c r="H57" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2218,11 +2392,14 @@
       <c r="F58">
         <v>63</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G58">
+        <v>63</v>
+      </c>
+      <c r="H58" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2241,11 +2418,14 @@
       <c r="F59">
         <v>64</v>
       </c>
-      <c r="G59" t="s">
+      <c r="G59">
+        <v>64</v>
+      </c>
+      <c r="H59" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2264,11 +2444,14 @@
       <c r="F60">
         <v>65</v>
       </c>
-      <c r="G60" t="s">
+      <c r="G60">
+        <v>65</v>
+      </c>
+      <c r="H60" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2287,11 +2470,14 @@
       <c r="F61">
         <v>66</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G61">
+        <v>66</v>
+      </c>
+      <c r="H61" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2310,11 +2496,14 @@
       <c r="F62">
         <v>68</v>
       </c>
-      <c r="G62" t="s">
+      <c r="G62">
+        <v>68</v>
+      </c>
+      <c r="H62" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2333,11 +2522,14 @@
       <c r="F63">
         <v>69</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G63">
+        <v>69</v>
+      </c>
+      <c r="H63" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2356,11 +2548,14 @@
       <c r="F64">
         <v>70</v>
       </c>
-      <c r="G64" t="s">
+      <c r="G64">
+        <v>70</v>
+      </c>
+      <c r="H64" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2379,11 +2574,14 @@
       <c r="F65">
         <v>71</v>
       </c>
-      <c r="G65" t="s">
+      <c r="G65">
+        <v>71</v>
+      </c>
+      <c r="H65" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2402,11 +2600,14 @@
       <c r="F66">
         <v>72</v>
       </c>
-      <c r="G66" t="s">
+      <c r="G66">
+        <v>72</v>
+      </c>
+      <c r="H66" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2425,11 +2626,14 @@
       <c r="F67">
         <v>73</v>
       </c>
-      <c r="G67" t="s">
+      <c r="G67">
+        <v>73</v>
+      </c>
+      <c r="H67" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2448,11 +2652,14 @@
       <c r="F68">
         <v>74</v>
       </c>
-      <c r="G68" t="s">
+      <c r="G68">
+        <v>74</v>
+      </c>
+      <c r="H68" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2471,11 +2678,14 @@
       <c r="F69">
         <v>75</v>
       </c>
-      <c r="G69" t="s">
+      <c r="G69">
+        <v>75</v>
+      </c>
+      <c r="H69" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2494,11 +2704,14 @@
       <c r="F70">
         <v>77</v>
       </c>
-      <c r="G70" t="s">
+      <c r="G70">
+        <v>77</v>
+      </c>
+      <c r="H70" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2517,11 +2730,14 @@
       <c r="F71">
         <v>78</v>
       </c>
-      <c r="G71" t="s">
+      <c r="G71">
+        <v>78</v>
+      </c>
+      <c r="H71" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2540,11 +2756,14 @@
       <c r="F72">
         <v>79</v>
       </c>
-      <c r="G72" t="s">
+      <c r="G72">
+        <v>79</v>
+      </c>
+      <c r="H72" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2563,11 +2782,14 @@
       <c r="F73">
         <v>80</v>
       </c>
-      <c r="G73" t="s">
+      <c r="G73">
+        <v>80</v>
+      </c>
+      <c r="H73" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2586,11 +2808,14 @@
       <c r="F74">
         <v>81</v>
       </c>
-      <c r="G74" t="s">
+      <c r="G74">
+        <v>81</v>
+      </c>
+      <c r="H74" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2609,11 +2834,14 @@
       <c r="F75">
         <v>82</v>
       </c>
-      <c r="G75" t="s">
+      <c r="G75">
+        <v>82</v>
+      </c>
+      <c r="H75" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2632,11 +2860,14 @@
       <c r="F76">
         <v>84</v>
       </c>
-      <c r="G76" t="s">
+      <c r="G76">
+        <v>84</v>
+      </c>
+      <c r="H76" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2655,11 +2886,14 @@
       <c r="F77">
         <v>85</v>
       </c>
-      <c r="G77" t="s">
+      <c r="G77">
+        <v>85</v>
+      </c>
+      <c r="H77" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2678,11 +2912,14 @@
       <c r="F78">
         <v>86</v>
       </c>
-      <c r="G78" t="s">
+      <c r="G78">
+        <v>86</v>
+      </c>
+      <c r="H78" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2701,11 +2938,14 @@
       <c r="F79">
         <v>87</v>
       </c>
-      <c r="G79" t="s">
+      <c r="G79">
+        <v>87</v>
+      </c>
+      <c r="H79" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2724,11 +2964,14 @@
       <c r="F80">
         <v>88</v>
       </c>
-      <c r="G80" t="s">
+      <c r="G80">
+        <v>88</v>
+      </c>
+      <c r="H80" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2747,11 +2990,14 @@
       <c r="F81">
         <v>90</v>
       </c>
-      <c r="G81" t="s">
+      <c r="G81">
+        <v>90</v>
+      </c>
+      <c r="H81" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2770,11 +3016,14 @@
       <c r="F82">
         <v>91</v>
       </c>
-      <c r="G82" t="s">
+      <c r="G82">
+        <v>91</v>
+      </c>
+      <c r="H82" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2793,11 +3042,14 @@
       <c r="F83">
         <v>92</v>
       </c>
-      <c r="G83" t="s">
+      <c r="G83">
+        <v>92</v>
+      </c>
+      <c r="H83" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2816,11 +3068,14 @@
       <c r="F84">
         <v>93</v>
       </c>
-      <c r="G84" t="s">
+      <c r="G84">
+        <v>93</v>
+      </c>
+      <c r="H84" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2839,11 +3094,14 @@
       <c r="F85">
         <v>94</v>
       </c>
-      <c r="G85" t="s">
+      <c r="G85">
+        <v>94</v>
+      </c>
+      <c r="H85" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2862,11 +3120,14 @@
       <c r="F86">
         <v>95</v>
       </c>
-      <c r="G86" t="s">
+      <c r="G86">
+        <v>95</v>
+      </c>
+      <c r="H86" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2885,11 +3146,14 @@
       <c r="F87">
         <v>96</v>
       </c>
-      <c r="G87" t="s">
+      <c r="G87">
+        <v>96</v>
+      </c>
+      <c r="H87" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2908,11 +3172,14 @@
       <c r="F88">
         <v>97</v>
       </c>
-      <c r="G88" t="s">
+      <c r="G88">
+        <v>97</v>
+      </c>
+      <c r="H88" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>87</v>
       </c>
@@ -2929,13 +3196,16 @@
         <v>33</v>
       </c>
       <c r="F89">
+        <v>97</v>
+      </c>
+      <c r="G89">
         <v>98</v>
       </c>
-      <c r="G89" t="s">
+      <c r="H89" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>88</v>
       </c>
@@ -2954,7 +3224,10 @@
       <c r="F90">
         <v>99</v>
       </c>
-      <c r="G90" t="s">
+      <c r="G90">
+        <v>99</v>
+      </c>
+      <c r="H90" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>

<commit_message>
avance ID2 a CAENES_1d
</commit_message>
<xml_diff>
--- a/input/data/dt/CAE_DT_armonizado.xlsx
+++ b/input/data/dt/CAE_DT_armonizado.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\proyecto_sindicalizacion\input\data\dt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379BE031-4C37-4D1F-A284-B5CECE403CB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2784CA46-7310-4831-8B4E-4DEC04B42DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-1335" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="125">
   <si>
     <t>id_cae2</t>
   </si>
@@ -405,6 +405,9 @@
   </si>
   <si>
     <t>codigoactividad</t>
+  </si>
+  <si>
+    <t>CAENES_1d_4</t>
   </si>
 </sst>
 </file>
@@ -893,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42:D90"/>
+    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36:I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -904,7 +907,7 @@
     <col min="7" max="7" width="13.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -927,10 +930,13 @@
         <v>92</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -955,8 +961,11 @@
       <c r="H2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -981,8 +990,11 @@
       <c r="H3" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1007,8 +1019,11 @@
       <c r="H4" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1033,8 +1048,11 @@
       <c r="H5" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1059,8 +1077,11 @@
       <c r="H6" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1085,8 +1106,11 @@
       <c r="H7" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1111,8 +1135,11 @@
       <c r="H8" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1137,8 +1164,11 @@
       <c r="H9" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1163,8 +1193,11 @@
       <c r="H10" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1189,8 +1222,11 @@
       <c r="H11" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1215,8 +1251,11 @@
       <c r="H12" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1241,8 +1280,11 @@
       <c r="H13" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I13" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1267,8 +1309,11 @@
       <c r="H14" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1293,8 +1338,11 @@
       <c r="H15" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1319,8 +1367,11 @@
       <c r="H16" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I16" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1345,8 +1396,11 @@
       <c r="H17" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1371,8 +1425,11 @@
       <c r="H18" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I18" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1397,8 +1454,11 @@
       <c r="H19" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I19" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1423,8 +1483,11 @@
       <c r="H20" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1449,8 +1512,11 @@
       <c r="H21" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I21" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1475,8 +1541,11 @@
       <c r="H22" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I22" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1501,8 +1570,11 @@
       <c r="H23" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I23" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1527,8 +1599,11 @@
       <c r="H24" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I24" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1553,8 +1628,11 @@
       <c r="H25" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I25" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1579,8 +1657,11 @@
       <c r="H26" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I26" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1605,8 +1686,11 @@
       <c r="H27" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1631,8 +1715,11 @@
       <c r="H28" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1657,8 +1744,11 @@
       <c r="H29" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I29" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1683,8 +1773,11 @@
       <c r="H30" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I30" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1709,8 +1802,11 @@
       <c r="H31" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I31" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1733,6 +1829,9 @@
         <v>31</v>
       </c>
       <c r="H32" t="s">
+        <v>113</v>
+      </c>
+      <c r="I32" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1761,6 +1860,9 @@
       <c r="H33" t="s">
         <v>113</v>
       </c>
+      <c r="I33" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34">
@@ -1787,6 +1889,9 @@
       <c r="H34" t="s">
         <v>113</v>
       </c>
+      <c r="I34" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35">
@@ -1813,6 +1918,9 @@
       <c r="H35" t="s">
         <v>112</v>
       </c>
+      <c r="I35" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36">
@@ -1839,6 +1947,9 @@
       <c r="H36" t="s">
         <v>105</v>
       </c>
+      <c r="I36" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37">
@@ -1865,6 +1976,9 @@
       <c r="H37" t="s">
         <v>105</v>
       </c>
+      <c r="I37" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38">
@@ -1891,6 +2005,9 @@
       <c r="H38" t="s">
         <v>105</v>
       </c>
+      <c r="I38" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39">
@@ -1917,6 +2034,9 @@
       <c r="H39" t="s">
         <v>105</v>
       </c>
+      <c r="I39" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40">
@@ -1943,6 +2063,9 @@
       <c r="H40" t="s">
         <v>106</v>
       </c>
+      <c r="I40" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41">
@@ -1969,6 +2092,9 @@
       <c r="H41" t="s">
         <v>106</v>
       </c>
+      <c r="I41" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42">
@@ -1995,9 +2121,8 @@
       <c r="H42" t="s">
         <v>106</v>
       </c>
-      <c r="I42">
-        <f>D42-1</f>
-        <v>16</v>
+      <c r="I42" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
@@ -2025,9 +2150,8 @@
       <c r="H43" t="s">
         <v>115</v>
       </c>
-      <c r="I43">
-        <f t="shared" ref="I43:I90" si="0">D43-1</f>
-        <v>17</v>
+      <c r="I43" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
@@ -2055,9 +2179,8 @@
       <c r="H44" t="s">
         <v>115</v>
       </c>
-      <c r="I44">
-        <f t="shared" si="0"/>
-        <v>18</v>
+      <c r="I44" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
@@ -2085,9 +2208,8 @@
       <c r="H45" t="s">
         <v>115</v>
       </c>
-      <c r="I45">
-        <f t="shared" si="0"/>
-        <v>19</v>
+      <c r="I45" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
@@ -2115,9 +2237,8 @@
       <c r="H46" t="s">
         <v>116</v>
       </c>
-      <c r="I46">
-        <f t="shared" si="0"/>
-        <v>20</v>
+      <c r="I46" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
@@ -2145,9 +2266,8 @@
       <c r="H47" t="s">
         <v>116</v>
       </c>
-      <c r="I47">
-        <f t="shared" si="0"/>
-        <v>21</v>
+      <c r="I47" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
@@ -2175,9 +2295,8 @@
       <c r="H48" t="s">
         <v>116</v>
       </c>
-      <c r="I48">
-        <f t="shared" si="0"/>
-        <v>21</v>
+      <c r="I48" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
@@ -2205,9 +2324,8 @@
       <c r="H49" t="s">
         <v>116</v>
       </c>
-      <c r="I49">
-        <f t="shared" si="0"/>
-        <v>22</v>
+      <c r="I49" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
@@ -2235,9 +2353,8 @@
       <c r="H50" t="s">
         <v>116</v>
       </c>
-      <c r="I50">
-        <f t="shared" si="0"/>
-        <v>22</v>
+      <c r="I50" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
@@ -2265,9 +2382,8 @@
       <c r="H51" t="s">
         <v>107</v>
       </c>
-      <c r="I51">
-        <f t="shared" si="0"/>
-        <v>23</v>
+      <c r="I51" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
@@ -2295,9 +2411,8 @@
       <c r="H52" t="s">
         <v>107</v>
       </c>
-      <c r="I52">
-        <f t="shared" si="0"/>
-        <v>24</v>
+      <c r="I52" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
@@ -2325,9 +2440,8 @@
       <c r="H53" t="s">
         <v>117</v>
       </c>
-      <c r="I53">
-        <f t="shared" si="0"/>
-        <v>25</v>
+      <c r="I53" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
@@ -2355,9 +2469,8 @@
       <c r="H54" t="s">
         <v>117</v>
       </c>
-      <c r="I54">
-        <f t="shared" si="0"/>
-        <v>25</v>
+      <c r="I54" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
@@ -2385,9 +2498,8 @@
       <c r="H55" t="s">
         <v>117</v>
       </c>
-      <c r="I55">
-        <f t="shared" si="0"/>
-        <v>25</v>
+      <c r="I55" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
@@ -2415,9 +2527,8 @@
       <c r="H56" t="s">
         <v>117</v>
       </c>
-      <c r="I56">
-        <f t="shared" si="0"/>
-        <v>26</v>
+      <c r="I56" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
@@ -2445,9 +2556,8 @@
       <c r="H57" t="s">
         <v>117</v>
       </c>
-      <c r="I57">
-        <f t="shared" si="0"/>
-        <v>27</v>
+      <c r="I57" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
@@ -2475,9 +2585,8 @@
       <c r="H58" t="s">
         <v>117</v>
       </c>
-      <c r="I58">
-        <f t="shared" si="0"/>
-        <v>27</v>
+      <c r="I58" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
@@ -2505,9 +2614,8 @@
       <c r="H59" t="s">
         <v>118</v>
       </c>
-      <c r="I59">
-        <f t="shared" si="0"/>
-        <v>28</v>
+      <c r="I59" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
@@ -2535,9 +2643,8 @@
       <c r="H60" t="s">
         <v>118</v>
       </c>
-      <c r="I60">
-        <f t="shared" si="0"/>
-        <v>28</v>
+      <c r="I60" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
@@ -2565,9 +2672,8 @@
       <c r="H61" t="s">
         <v>118</v>
       </c>
-      <c r="I61">
-        <f t="shared" si="0"/>
-        <v>28</v>
+      <c r="I61" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
@@ -2595,9 +2701,8 @@
       <c r="H62" t="s">
         <v>114</v>
       </c>
-      <c r="I62">
-        <f t="shared" si="0"/>
-        <v>29</v>
+      <c r="I62" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
@@ -2625,9 +2730,8 @@
       <c r="H63" t="s">
         <v>119</v>
       </c>
-      <c r="I63">
-        <f t="shared" si="0"/>
-        <v>30</v>
+      <c r="I63" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
@@ -2655,9 +2759,8 @@
       <c r="H64" t="s">
         <v>119</v>
       </c>
-      <c r="I64">
-        <f t="shared" si="0"/>
-        <v>30</v>
+      <c r="I64" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
@@ -2685,9 +2788,8 @@
       <c r="H65" t="s">
         <v>119</v>
       </c>
-      <c r="I65">
-        <f t="shared" si="0"/>
-        <v>30</v>
+      <c r="I65" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
@@ -2715,9 +2817,8 @@
       <c r="H66" t="s">
         <v>119</v>
       </c>
-      <c r="I66">
-        <f t="shared" si="0"/>
-        <v>30</v>
+      <c r="I66" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
@@ -2745,9 +2846,8 @@
       <c r="H67" t="s">
         <v>119</v>
       </c>
-      <c r="I67">
-        <f t="shared" si="0"/>
-        <v>30</v>
+      <c r="I67" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.35">
@@ -2775,9 +2875,8 @@
       <c r="H68" t="s">
         <v>119</v>
       </c>
-      <c r="I68">
-        <f t="shared" si="0"/>
-        <v>30</v>
+      <c r="I68" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
@@ -2805,9 +2904,8 @@
       <c r="H69" t="s">
         <v>119</v>
       </c>
-      <c r="I69">
-        <f t="shared" si="0"/>
-        <v>30</v>
+      <c r="I69" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
@@ -2835,9 +2933,8 @@
       <c r="H70" t="s">
         <v>2</v>
       </c>
-      <c r="I70">
-        <f t="shared" si="0"/>
-        <v>31</v>
+      <c r="I70" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
@@ -2865,9 +2962,8 @@
       <c r="H71" t="s">
         <v>2</v>
       </c>
-      <c r="I71">
-        <f t="shared" si="0"/>
-        <v>31</v>
+      <c r="I71" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.35">
@@ -2895,9 +2991,8 @@
       <c r="H72" t="s">
         <v>2</v>
       </c>
-      <c r="I72">
-        <f t="shared" si="0"/>
-        <v>31</v>
+      <c r="I72" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.35">
@@ -2925,9 +3020,8 @@
       <c r="H73" t="s">
         <v>2</v>
       </c>
-      <c r="I73">
-        <f t="shared" si="0"/>
-        <v>31</v>
+      <c r="I73" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
@@ -2955,9 +3049,8 @@
       <c r="H74" t="s">
         <v>2</v>
       </c>
-      <c r="I74">
-        <f t="shared" si="0"/>
-        <v>31</v>
+      <c r="I74" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.35">
@@ -2985,9 +3078,8 @@
       <c r="H75" t="s">
         <v>2</v>
       </c>
-      <c r="I75">
-        <f t="shared" si="0"/>
-        <v>31</v>
+      <c r="I75" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.35">
@@ -3015,9 +3107,8 @@
       <c r="H76" t="s">
         <v>111</v>
       </c>
-      <c r="I76">
-        <f t="shared" si="0"/>
-        <v>32</v>
+      <c r="I76" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.35">
@@ -3045,9 +3136,8 @@
       <c r="H77" t="s">
         <v>104</v>
       </c>
-      <c r="I77">
-        <f t="shared" si="0"/>
-        <v>33</v>
+      <c r="I77" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.35">
@@ -3075,9 +3165,8 @@
       <c r="H78" t="s">
         <v>120</v>
       </c>
-      <c r="I78">
-        <f t="shared" si="0"/>
-        <v>34</v>
+      <c r="I78" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.35">
@@ -3105,9 +3194,8 @@
       <c r="H79" t="s">
         <v>120</v>
       </c>
-      <c r="I79">
-        <f t="shared" si="0"/>
-        <v>35</v>
+      <c r="I79" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.35">
@@ -3135,9 +3223,8 @@
       <c r="H80" t="s">
         <v>120</v>
       </c>
-      <c r="I80">
-        <f t="shared" si="0"/>
-        <v>36</v>
+      <c r="I80" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
@@ -3165,9 +3252,8 @@
       <c r="H81" t="s">
         <v>109</v>
       </c>
-      <c r="I81">
-        <f t="shared" si="0"/>
-        <v>37</v>
+      <c r="I81" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
@@ -3195,9 +3281,8 @@
       <c r="H82" t="s">
         <v>109</v>
       </c>
-      <c r="I82">
-        <f t="shared" si="0"/>
-        <v>37</v>
+      <c r="I82" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
@@ -3225,9 +3310,8 @@
       <c r="H83" t="s">
         <v>109</v>
       </c>
-      <c r="I83">
-        <f t="shared" si="0"/>
-        <v>37</v>
+      <c r="I83" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.35">
@@ -3255,9 +3339,8 @@
       <c r="H84" t="s">
         <v>109</v>
       </c>
-      <c r="I84">
-        <f t="shared" si="0"/>
-        <v>37</v>
+      <c r="I84" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.35">
@@ -3285,9 +3368,8 @@
       <c r="H85" t="s">
         <v>103</v>
       </c>
-      <c r="I85">
-        <f t="shared" si="0"/>
-        <v>38</v>
+      <c r="I85" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.35">
@@ -3315,9 +3397,8 @@
       <c r="H86" t="s">
         <v>103</v>
       </c>
-      <c r="I86">
-        <f t="shared" si="0"/>
-        <v>39</v>
+      <c r="I86" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
@@ -3345,9 +3426,8 @@
       <c r="H87" t="s">
         <v>103</v>
       </c>
-      <c r="I87">
-        <f t="shared" si="0"/>
-        <v>40</v>
+      <c r="I87" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.35">
@@ -3375,9 +3455,8 @@
       <c r="H88" t="s">
         <v>103</v>
       </c>
-      <c r="I88">
-        <f t="shared" si="0"/>
-        <v>40</v>
+      <c r="I88" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
@@ -3405,9 +3484,8 @@
       <c r="H89" t="s">
         <v>103</v>
       </c>
-      <c r="I89">
-        <f t="shared" si="0"/>
-        <v>40</v>
+      <c r="I89" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.35">
@@ -3435,9 +3513,8 @@
       <c r="H90" t="s">
         <v>110</v>
       </c>
-      <c r="I90">
-        <f t="shared" si="0"/>
-        <v>41</v>
+      <c r="I90" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
falta actualizar datos ene
</commit_message>
<xml_diff>
--- a/input/data/dt/CAE_DT_armonizado.xlsx
+++ b/input/data/dt/CAE_DT_armonizado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\proyecto_sindicalizacion\input\data\dt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2784CA46-7310-4831-8B4E-4DEC04B42DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0820890F-B867-42AA-9539-BCE9E81486B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -896,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36:I39"/>
+    <sheetView tabSelected="1" topLeftCell="B73" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I90" sqref="I90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3514,7 +3514,7 @@
         <v>110</v>
       </c>
       <c r="I90" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
graficos anuario y rraa DT
</commit_message>
<xml_diff>
--- a/input/data/dt/CAE_DT_armonizado.xlsx
+++ b/input/data/dt/CAE_DT_armonizado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\proyecto_sindicalizacion\input\data\dt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0820890F-B867-42AA-9539-BCE9E81486B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C392762-0854-4078-B890-C9E79E3D0541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="129">
   <si>
     <t>id_cae2</t>
   </si>
@@ -408,6 +408,18 @@
   </si>
   <si>
     <t>CAENES_1d_4</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>HJ</t>
+  </si>
+  <si>
+    <t>LMN</t>
+  </si>
+  <si>
+    <t>RS</t>
   </si>
 </sst>
 </file>
@@ -565,7 +577,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -590,6 +602,7 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -896,8 +909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B73" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I90" sqref="I90"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I82" sqref="I82:I89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1919,7 +1932,7 @@
         <v>112</v>
       </c>
       <c r="I35" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
@@ -1948,7 +1961,7 @@
         <v>105</v>
       </c>
       <c r="I36" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
@@ -1977,7 +1990,7 @@
         <v>105</v>
       </c>
       <c r="I37" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
@@ -2006,7 +2019,7 @@
         <v>105</v>
       </c>
       <c r="I38" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
@@ -2035,7 +2048,7 @@
         <v>105</v>
       </c>
       <c r="I39" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
@@ -2238,7 +2251,7 @@
         <v>116</v>
       </c>
       <c r="I46" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
@@ -2267,7 +2280,7 @@
         <v>116</v>
       </c>
       <c r="I47" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
@@ -2296,7 +2309,7 @@
         <v>116</v>
       </c>
       <c r="I48" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
@@ -2325,7 +2338,7 @@
         <v>116</v>
       </c>
       <c r="I49" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
@@ -2354,7 +2367,7 @@
         <v>116</v>
       </c>
       <c r="I50" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
@@ -2441,7 +2454,7 @@
         <v>117</v>
       </c>
       <c r="I53" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
@@ -2470,7 +2483,7 @@
         <v>117</v>
       </c>
       <c r="I54" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
@@ -2499,7 +2512,7 @@
         <v>117</v>
       </c>
       <c r="I55" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
@@ -2528,7 +2541,7 @@
         <v>117</v>
       </c>
       <c r="I56" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
@@ -2557,7 +2570,7 @@
         <v>117</v>
       </c>
       <c r="I57" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
@@ -2586,7 +2599,7 @@
         <v>117</v>
       </c>
       <c r="I58" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
@@ -2702,7 +2715,7 @@
         <v>114</v>
       </c>
       <c r="I62" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
@@ -2731,7 +2744,7 @@
         <v>119</v>
       </c>
       <c r="I63" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
@@ -2760,7 +2773,7 @@
         <v>119</v>
       </c>
       <c r="I64" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
@@ -2789,7 +2802,7 @@
         <v>119</v>
       </c>
       <c r="I65" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
@@ -2818,7 +2831,7 @@
         <v>119</v>
       </c>
       <c r="I66" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
@@ -2847,7 +2860,7 @@
         <v>119</v>
       </c>
       <c r="I67" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.35">
@@ -2876,7 +2889,7 @@
         <v>119</v>
       </c>
       <c r="I68" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
@@ -2905,7 +2918,7 @@
         <v>119</v>
       </c>
       <c r="I69" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
@@ -2934,7 +2947,7 @@
         <v>2</v>
       </c>
       <c r="I70" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
@@ -2963,7 +2976,7 @@
         <v>2</v>
       </c>
       <c r="I71" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.35">
@@ -2992,7 +3005,7 @@
         <v>2</v>
       </c>
       <c r="I72" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.35">
@@ -3021,7 +3034,7 @@
         <v>2</v>
       </c>
       <c r="I73" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
@@ -3050,7 +3063,7 @@
         <v>2</v>
       </c>
       <c r="I74" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.35">
@@ -3079,7 +3092,7 @@
         <v>2</v>
       </c>
       <c r="I75" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.35">
@@ -3253,7 +3266,7 @@
         <v>109</v>
       </c>
       <c r="I81" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
@@ -3281,8 +3294,8 @@
       <c r="H82" t="s">
         <v>109</v>
       </c>
-      <c r="I82" t="s">
-        <v>109</v>
+      <c r="I82" s="22" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
@@ -3310,8 +3323,8 @@
       <c r="H83" t="s">
         <v>109</v>
       </c>
-      <c r="I83" t="s">
-        <v>109</v>
+      <c r="I83" s="22" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.35">
@@ -3339,8 +3352,8 @@
       <c r="H84" t="s">
         <v>109</v>
       </c>
-      <c r="I84" t="s">
-        <v>109</v>
+      <c r="I84" s="22" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.35">
@@ -3368,8 +3381,8 @@
       <c r="H85" t="s">
         <v>103</v>
       </c>
-      <c r="I85" t="s">
-        <v>103</v>
+      <c r="I85" s="22" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.35">
@@ -3397,8 +3410,8 @@
       <c r="H86" t="s">
         <v>103</v>
       </c>
-      <c r="I86" t="s">
-        <v>103</v>
+      <c r="I86" s="22" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
@@ -3426,8 +3439,8 @@
       <c r="H87" t="s">
         <v>103</v>
       </c>
-      <c r="I87" t="s">
-        <v>103</v>
+      <c r="I87" s="22" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.35">
@@ -3455,8 +3468,8 @@
       <c r="H88" t="s">
         <v>103</v>
       </c>
-      <c r="I88" t="s">
-        <v>103</v>
+      <c r="I88" s="22" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
@@ -3484,8 +3497,8 @@
       <c r="H89" t="s">
         <v>103</v>
       </c>
-      <c r="I89" t="s">
-        <v>103</v>
+      <c r="I89" s="22" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>